<commit_message>
Added extra test cells added
</commit_message>
<xml_diff>
--- a/apachepoi-xssf/Test01.xlsx
+++ b/apachepoi-xssf/Test01.xlsx
@@ -5,17 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>"text 1"</t>
   </si>
@@ -30,6 +35,57 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>t ext</t>
+  </si>
+  <si>
+    <t>te xt</t>
+  </si>
+  <si>
+    <t>tex t</t>
+  </si>
+  <si>
+    <t>t ex t</t>
+  </si>
+  <si>
+    <t>t
+ext</t>
+  </si>
+  <si>
+    <t>te
+xt</t>
+  </si>
+  <si>
+    <t>tex
+t</t>
+  </si>
+  <si>
+    <t>te"xt</t>
+  </si>
+  <si>
+    <t>te,xt</t>
+  </si>
+  <si>
+    <t>te " xt</t>
+  </si>
+  <si>
+    <t>te , xt</t>
+  </si>
+  <si>
+    <t>“te-xt”</t>
+  </si>
+  <si>
+    <t>t e – st</t>
+  </si>
+  <si>
+    <t>te\st</t>
+  </si>
+  <si>
+    <t>te\\st</t>
   </si>
 </sst>
 </file>
@@ -44,6 +100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,9 +160,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -123,19 +184,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -177,7 +237,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -192,6 +252,9 @@
       </c>
       <c r="D4" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -245,7 +308,13 @@
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">D3</f>
-        <v>text</v>
+        <v>test</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,9 +330,61 @@
         <f aca="false">C4</f>
         <v>text</v>
       </c>
-      <c r="D8" s="0" t="str">
-        <f aca="false">D4</f>
-        <v>text</v>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extend tests and fixes
</commit_message>
<xml_diff>
--- a/apachepoi-xssf/Test01.xlsx
+++ b/apachepoi-xssf/Test01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>"text 1"</t>
   </si>
@@ -74,18 +74,6 @@
   </si>
   <si>
     <t>te , xt</t>
-  </si>
-  <si>
-    <t>“te-xt”</t>
-  </si>
-  <si>
-    <t>t e – st</t>
-  </si>
-  <si>
-    <t>te\st</t>
-  </si>
-  <si>
-    <t>te\\st</t>
   </si>
 </sst>
 </file>
@@ -187,16 +175,13 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -371,20 +356,6 @@
       </c>
       <c r="D11" s="0" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to date and time formatting
</commit_message>
<xml_diff>
--- a/apachepoi-xssf/Test01.xlsx
+++ b/apachepoi-xssf/Test01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -80,8 +80,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="HH:MM"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -148,13 +151,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -175,13 +190,18 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:11"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -356,6 +376,20 @@
       </c>
       <c r="D11" s="0" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>23349</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>4011</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0.583333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>